<commit_message>
fixed results to use integers up to 100 rather than just 10
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,18 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/durst/dev/18-19/matrix_multiplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E30F550-092D-6C4B-9615-4914E7BC76BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE4D64-7C09-9E46-BDB4-BF379D9CCA33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="times" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">times!$I$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">times!$I$2:$I$17</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">times!$J$2:$J$17</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
@@ -126,26 +121,26 @@
     <t>522299d</t>
   </si>
   <si>
-    <t>20190103-110955</t>
-  </si>
-  <si>
-    <t>885dc4b</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date and Time </t>
   </si>
   <si>
     <t>my implementation time / numpy time</t>
+  </si>
+  <si>
+    <t>20190103-120527</t>
+  </si>
+  <si>
+    <t>c75e8b7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -279,6 +274,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -622,10 +623,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -822,7 +824,7 @@
                   <c:v>43468.461875000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43468.465219907404</c:v>
+                  <c:v>43468.503784722219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,7 +881,7 @@
                   <c:v>2.1702127659574466</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20520866018198933</c:v>
+                  <c:v>0.19011056511056512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2086,11 +2088,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2125,10 +2127,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2644,37 +2646,40 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17">
-        <v>1678</v>
+        <v>1605</v>
       </c>
       <c r="D17">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="E17">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="F17">
-        <v>1622</v>
+        <v>1616</v>
       </c>
       <c r="G17">
-        <v>3187</v>
+        <v>3256</v>
       </c>
       <c r="H17">
-        <v>654</v>
+        <v>619</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>0.20520866018198933</v>
+        <v>0.19011056511056512</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="1"/>
-        <v>43468.465219907404</v>
-      </c>
+        <v>43468.503784722219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>